<commit_message>
actually using data now
</commit_message>
<xml_diff>
--- a/SCE_ClientInfo_Template.xlsx
+++ b/SCE_ClientInfo_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\GitHub\2023-01_Team6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA156492-A8C4-4685-B2E7-B726DC49E48D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC1CD4A-2705-4282-8487-9AD9F5D93ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5025" yWindow="2190" windowWidth="21600" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="11">
   <si>
     <t>Term #</t>
   </si>
@@ -409,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,7 +440,7 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -451,7 +451,7 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -484,7 +484,7 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -495,7 +495,7 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -682,14 +682,6 @@
         <v>9</v>
       </c>
       <c r="C24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed a bug were an infinite loop would occure due to time loss that could not be accounted for in cohort creation. Cohort creation now has the ability to estimte time loss in a schedule to prevent this in the future
</commit_message>
<xml_diff>
--- a/SCE_ClientInfo_Template.xlsx
+++ b/SCE_ClientInfo_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\GitHub\2023-01_Team6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conla\PycharmProjects\2023-01_Team6-Conlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC1CD4A-2705-4282-8487-9AD9F5D93ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF24E62-E316-452C-BDB7-A3531E22EDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -411,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,7 +440,7 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -627,7 +627,7 @@
         <v>4</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -671,7 +671,7 @@
         <v>8</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -682,7 +682,7 @@
         <v>9</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finnaly fixed issue of overllaping scheduling, however scheduling is still ineffcient
</commit_message>
<xml_diff>
--- a/SCE_ClientInfo_Template.xlsx
+++ b/SCE_ClientInfo_Template.xlsx
@@ -8,15 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conla\PycharmProjects\2023-01_Team6-Conlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF24E62-E316-452C-BDB7-A3531E22EDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1537660D-6AA0-4A48-B457-1111632D3043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="2925" windowWidth="21600" windowHeight="10140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -411,8 +422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,7 +451,7 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>40</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -451,7 +462,7 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>30</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -462,7 +473,7 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -473,7 +484,7 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -484,7 +495,7 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -495,7 +506,7 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -627,7 +638,7 @@
         <v>4</v>
       </c>
       <c r="C19">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -671,7 +682,7 @@
         <v>8</v>
       </c>
       <c r="C23">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -682,7 +693,7 @@
         <v>9</v>
       </c>
       <c r="C24">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added functionality to spinners
</commit_message>
<xml_diff>
--- a/SCE_ClientInfo_Template.xlsx
+++ b/SCE_ClientInfo_Template.xlsx
@@ -5,29 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\GitHub\2023-01_Team6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conla\PycharmProjects\2023-01_Team6-Conlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B057AA-64FA-4DF0-9A28-9E94C0C37AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF24E62-E316-452C-BDB7-A3531E22EDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -422,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,7 +440,7 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -462,7 +451,7 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>80</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -473,7 +462,7 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -484,7 +473,7 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -495,7 +484,7 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -506,7 +495,7 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -638,7 +627,7 @@
         <v>4</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -682,7 +671,7 @@
         <v>8</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -693,7 +682,7 @@
         <v>9</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added error reporting to cohort creation so that the user can know what issue occured and what kind of classrooms are needed for that many students
</commit_message>
<xml_diff>
--- a/SCE_ClientInfo_Template.xlsx
+++ b/SCE_ClientInfo_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conla\PycharmProjects\2023-01_Team6-Conlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1537660D-6AA0-4A48-B457-1111632D3043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E092AB-8AC3-478A-985B-F583564A4F19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="735" yWindow="2925" windowWidth="21600" windowHeight="10140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -423,7 +423,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,7 +451,7 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>90</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>